<commit_message>
Licor and pollen tubes
</commit_message>
<xml_diff>
--- a/Output/Sporophytic_ANOVAresults.xlsx
+++ b/Output/Sporophytic_ANOVAresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Horsenettle\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A879B261-E77D-4489-AC46-1B6C7F326BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B128608-BE43-4DF2-B255-C83D65D91B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{267AA17C-9341-4022-A5B6-E72266D94439}"/>
+    <workbookView xWindow="9120" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{267AA17C-9341-4022-A5B6-E72266D94439}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Variable</t>
   </si>
@@ -72,9 +72,6 @@
     <t>na</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
     <t>Variation between genotype</t>
   </si>
   <si>
@@ -88,13 +85,16 @@
   </si>
   <si>
     <t>* Model including nested random effect had error with singular fit</t>
+  </si>
+  <si>
+    <t>Genotype Fixed Effect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +121,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -218,14 +223,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -235,23 +267,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC0EFEA-2DBB-471A-9F18-C998C9CAF029}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,282 +607,264 @@
     <col min="8" max="8" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G1" s="17"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="6">
         <v>3.4958</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="10">
-        <v>8.1189999999999998E-2</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="7">
+        <v>0.81189999999999996</v>
+      </c>
+      <c r="E3" s="8">
         <v>6.7530000000000007E-2</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="13">
         <v>3.1289999999999998E-2</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <v>5.5230000000000001E-2</v>
       </c>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
-        <v>2.141</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="B4" s="6">
+        <v>14.465999999999999</v>
+      </c>
+      <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="10">
-        <v>1.0186000000000001E-2</v>
+      <c r="D4" s="7">
+        <v>4.1672000000000001E-2</v>
       </c>
       <c r="E4" s="11">
-        <v>0.25409999999999999</v>
-      </c>
-      <c r="F4" s="19">
-        <v>3.4684999999999997E-5</v>
-      </c>
-      <c r="G4" s="15" t="s">
+        <v>1.9110000000000001E-4</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2.3270000000000001E-10</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="11">
-        <v>0.31990000000000002</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
-        <v>4.33</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="B5" s="6">
+        <v>3.5411999999999999</v>
+      </c>
+      <c r="C5" s="7">
         <v>1</v>
       </c>
-      <c r="D5" s="10">
-        <v>8.3193000000000003E-2</v>
-      </c>
-      <c r="E5" s="16">
-        <v>4.2689999999999999E-2</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0.85070000000000001</v>
-      </c>
-      <c r="G5" s="10">
-        <v>0.97230000000000005</v>
-      </c>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="7">
+        <v>6.3186000000000006E-2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>6.1339999999999999E-2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.48139999999999999</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
-        <v>59.670999999999999</v>
-      </c>
-      <c r="C6" s="13">
+      <c r="B6" s="9">
+        <v>66.614999999999995</v>
+      </c>
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D6" s="13">
-        <v>0.71423999999999999</v>
-      </c>
-      <c r="E6" s="17">
-        <v>4.1790000000000003E-10</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0.11115</v>
-      </c>
-      <c r="G6" s="20">
-        <v>2.9149999999999999E-2</v>
-      </c>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="10">
+        <v>0.64556999999999998</v>
+      </c>
+      <c r="E6" s="12">
+        <v>9.3229999999999998E-11</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.30470999999999998</v>
+      </c>
+      <c r="G6" s="21">
+        <v>9.2329999999999995E-2</v>
+      </c>
+      <c r="H6"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F11" s="4"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="9">
-        <v>1.6731</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B12" s="6">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="C12" s="7">
         <v>51</v>
       </c>
-      <c r="D12" s="10">
-        <v>3.8469999999999997E-2</v>
-      </c>
-      <c r="E12" s="16">
-        <v>9.2320000000000006E-3</v>
-      </c>
-      <c r="F12" s="18">
-        <v>2.2509999999999999E-2</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D12" s="7">
+        <v>3.823E-2</v>
+      </c>
+      <c r="E12" s="11">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <v>0.84750000000000003</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>51</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>4.4086999999999998E-3</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="8">
         <v>0.74880000000000002</v>
       </c>
-      <c r="F13" s="18">
-        <v>1.93E-4</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F13" s="22"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <v>1.0759000000000001</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>51</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="7">
         <v>2.0666E-2</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="8">
         <v>0.36070000000000002</v>
       </c>
-      <c r="F14" s="9">
-        <v>0.87109999999999999</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="9">
         <v>3.3290999999999999</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="10">
         <v>51</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <v>4.1488999999999998E-2</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="24">
         <v>2.7430000000000001E-9</v>
       </c>
-      <c r="F15" s="12">
-        <v>0.1293</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>